<commit_message>
se agregó contacto.php, capacitacion.php
</commit_message>
<xml_diff>
--- a/requerimientos/cronograma.xlsx
+++ b/requerimientos/cronograma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\oelt_v2\requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050433EE-AEC9-4781-987F-C92A9DABF47B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854693A1-14D3-470D-AED4-B2571DADDA1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,12 +174,12 @@
       <t xml:space="preserve">implementar página web Pestaña: solo vistas
 1. index (Inicio) (OK)
 2. Quienes somos. (OK)
-3. Servicios
-4. Catálogo
-5. Capacitación(cursos, diplomados)
+3. Servicios (OK)
+4. Catálogo (OK)
+5. Capacitación(cursos, diplomados)(OK)
 6. Intranet
 7. Aula Virtual
-8. Contacto
+8. Contacto(OK)
 </t>
     </r>
     <r>
@@ -989,7 +989,52 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="24" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="24" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="26" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="26" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -998,55 +1043,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="26" fillId="24" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="26" fillId="24" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="26" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="26" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="26" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1389,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="109" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,24 +1403,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1461,17 +1461,17 @@
       <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="53">
         <v>2</v>
       </c>
-      <c r="D5" s="44">
+      <c r="D5" s="41">
         <v>44321</v>
       </c>
-      <c r="E5" s="44">
+      <c r="E5" s="41">
         <v>44322</v>
       </c>
-      <c r="F5" s="46">
-        <v>0.25</v>
+      <c r="F5" s="43">
+        <v>0.5</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
@@ -1481,10 +1481,10 @@
       <c r="B6" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="47"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="44"/>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -1493,16 +1493,16 @@
       <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7" s="45">
         <v>2</v>
       </c>
-      <c r="D7" s="44">
+      <c r="D7" s="41">
         <v>44323</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="41">
         <v>44326</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1513,10 +1513,10 @@
       <c r="B8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="47"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="44"/>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -1525,16 +1525,16 @@
       <c r="B9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="53">
         <v>2</v>
       </c>
-      <c r="D9" s="59">
+      <c r="D9" s="54">
         <v>44327</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="54">
         <v>44328</v>
       </c>
-      <c r="F9" s="60">
+      <c r="F9" s="55">
         <v>0</v>
       </c>
     </row>
@@ -1545,10 +1545,10 @@
       <c r="B10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="60"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="55"/>
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -1557,10 +1557,10 @@
       <c r="B11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="60"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -1609,16 +1609,16 @@
       <c r="B14" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14" s="53">
         <v>2</v>
       </c>
-      <c r="D14" s="42">
+      <c r="D14" s="57">
         <v>44335</v>
       </c>
-      <c r="E14" s="44">
+      <c r="E14" s="41">
         <v>44336</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1629,10 +1629,10 @@
       <c r="B15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="41"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="47"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="58"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="44"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -1660,32 +1660,32 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="56" t="s">
+      <c r="C20" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="48" t="s">
+      <c r="D20" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="49"/>
-      <c r="F20" s="53">
+      <c r="E20" s="60"/>
+      <c r="F20" s="47">
         <f>SUM(F5:F15)/6</f>
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="C21" s="57"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="54"/>
+      <c r="F21" s="48"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
-      <c r="C22" s="58"/>
+      <c r="C22" s="52"/>
       <c r="D22" s="10">
         <f>D5</f>
         <v>44321</v>
@@ -1694,7 +1694,7 @@
         <f>E14</f>
         <v>44336</v>
       </c>
-      <c r="F22" s="55"/>
+      <c r="F22" s="49"/>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C25" s="33" t="s">
@@ -1706,6 +1706,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
@@ -1716,12 +1722,6 @@
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="F9:F11"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
@@ -1752,24 +1752,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G3" s="17"/>
@@ -1802,14 +1802,14 @@
         <v>1</v>
       </c>
       <c r="B5" s="9"/>
-      <c r="C5" s="51">
+      <c r="C5" s="45">
         <v>1</v>
       </c>
       <c r="D5" s="62">
         <v>44326</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="60">
+      <c r="E5" s="57"/>
+      <c r="F5" s="55">
         <v>0</v>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       <c r="C6" s="61"/>
       <c r="D6" s="63"/>
       <c r="E6" s="64"/>
-      <c r="F6" s="60"/>
+      <c r="F6" s="55"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -1831,31 +1831,31 @@
       <c r="C7" s="61"/>
       <c r="D7" s="63"/>
       <c r="E7" s="64"/>
-      <c r="F7" s="60"/>
+      <c r="F7" s="55"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>4</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="52"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="65"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="60"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="55"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>5</v>
       </c>
       <c r="B9" s="9"/>
-      <c r="C9" s="51">
+      <c r="C9" s="45">
         <v>1</v>
       </c>
       <c r="D9" s="62">
         <v>44327</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="60">
+      <c r="E9" s="57"/>
+      <c r="F9" s="55">
         <v>0</v>
       </c>
     </row>
@@ -1867,7 +1867,7 @@
       <c r="C10" s="61"/>
       <c r="D10" s="63"/>
       <c r="E10" s="64"/>
-      <c r="F10" s="60"/>
+      <c r="F10" s="55"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -1877,31 +1877,31 @@
       <c r="C11" s="61"/>
       <c r="D11" s="63"/>
       <c r="E11" s="64"/>
-      <c r="F11" s="60"/>
+      <c r="F11" s="55"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>8</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="52"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="65"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="60"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="55"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>9</v>
       </c>
       <c r="B13" s="9"/>
-      <c r="C13" s="51">
+      <c r="C13" s="45">
         <v>1</v>
       </c>
       <c r="D13" s="62">
         <v>44328</v>
       </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="60">
+      <c r="E13" s="57"/>
+      <c r="F13" s="55">
         <v>0</v>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       <c r="C14" s="61"/>
       <c r="D14" s="63"/>
       <c r="E14" s="64"/>
-      <c r="F14" s="60"/>
+      <c r="F14" s="55"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -1923,31 +1923,31 @@
       <c r="C15" s="61"/>
       <c r="D15" s="63"/>
       <c r="E15" s="64"/>
-      <c r="F15" s="60"/>
+      <c r="F15" s="55"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>12</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="52"/>
+      <c r="C16" s="46"/>
       <c r="D16" s="65"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="60"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="55"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>13</v>
       </c>
       <c r="B17" s="9"/>
-      <c r="C17" s="51">
+      <c r="C17" s="45">
         <v>1</v>
       </c>
       <c r="D17" s="62">
         <v>44329</v>
       </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="60">
+      <c r="E17" s="57"/>
+      <c r="F17" s="55">
         <v>0</v>
       </c>
     </row>
@@ -1959,7 +1959,7 @@
       <c r="C18" s="61"/>
       <c r="D18" s="63"/>
       <c r="E18" s="64"/>
-      <c r="F18" s="60"/>
+      <c r="F18" s="55"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -1969,31 +1969,31 @@
       <c r="C19" s="61"/>
       <c r="D19" s="63"/>
       <c r="E19" s="64"/>
-      <c r="F19" s="60"/>
+      <c r="F19" s="55"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>16</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="52"/>
+      <c r="C20" s="46"/>
       <c r="D20" s="65"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="60"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="55"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>13</v>
       </c>
       <c r="B21" s="9"/>
-      <c r="C21" s="51">
+      <c r="C21" s="45">
         <v>1</v>
       </c>
       <c r="D21" s="62">
         <v>44330</v>
       </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="60">
+      <c r="E21" s="57"/>
+      <c r="F21" s="55">
         <v>0</v>
       </c>
     </row>
@@ -2005,7 +2005,7 @@
       <c r="C22" s="61"/>
       <c r="D22" s="63"/>
       <c r="E22" s="64"/>
-      <c r="F22" s="60"/>
+      <c r="F22" s="55"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
@@ -2015,17 +2015,17 @@
       <c r="C23" s="61"/>
       <c r="D23" s="63"/>
       <c r="E23" s="64"/>
-      <c r="F23" s="60"/>
+      <c r="F23" s="55"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>16</v>
       </c>
       <c r="B24" s="7"/>
-      <c r="C24" s="52"/>
+      <c r="C24" s="46"/>
       <c r="D24" s="65"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="60"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="55"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
@@ -2054,32 +2054,32 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="56" t="s">
+      <c r="C29" s="50" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="15"/>
-      <c r="F29" s="53">
+      <c r="F29" s="47">
         <f>SUM(F5:F8)/6</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
-      <c r="C30" s="57"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="54"/>
+      <c r="F30" s="48"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
-      <c r="C31" s="58"/>
+      <c r="C31" s="52"/>
       <c r="D31" s="10">
         <f>D5</f>
         <v>44326</v>
@@ -2088,10 +2088,21 @@
         <f>D17</f>
         <v>44329</v>
       </c>
-      <c r="F31" s="55"/>
+      <c r="F31" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D21:E24"/>
+    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:E16"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:E20"/>
+    <mergeCell ref="F17:F20"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="D9:E12"/>
     <mergeCell ref="F9:F12"/>
@@ -2100,17 +2111,6 @@
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:E8"/>
     <mergeCell ref="F5:F8"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:E16"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:E20"/>
-    <mergeCell ref="F17:F20"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="D21:E24"/>
-    <mergeCell ref="F21:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se terminó con el item de capacitacion - diplomado
</commit_message>
<xml_diff>
--- a/requerimientos/cronograma.xlsx
+++ b/requerimientos/cronograma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\oelt_v2\requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854693A1-14D3-470D-AED4-B2571DADDA1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A22154-02B4-4E2F-BF79-50A12D4047CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Semana 1" sheetId="1" r:id="rId1"/>
@@ -177,7 +177,7 @@
 3. Servicios (OK)
 4. Catálogo (OK)
 5. Capacitación(cursos, diplomados)(OK)
-6. Intranet
+6. Intranet(OK)
 7. Aula Virtual
 8. Contacto(OK)
 </t>
@@ -989,6 +989,12 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1025,16 +1031,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="26" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1389,7 +1389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="109" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="109" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F7" sqref="F7:F8"/>
     </sheetView>
   </sheetViews>
@@ -1403,24 +1403,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1461,17 +1461,17 @@
       <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="53">
+      <c r="C5" s="42">
         <v>2</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="43">
         <v>44321</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="43">
         <v>44322</v>
       </c>
-      <c r="F5" s="43">
-        <v>0.5</v>
+      <c r="F5" s="45">
+        <v>0.7</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
@@ -1481,10 +1481,10 @@
       <c r="B6" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="53"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="44"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="46"/>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -1493,16 +1493,16 @@
       <c r="B7" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="47">
         <v>2</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="43">
         <v>44323</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="43">
         <v>44326</v>
       </c>
-      <c r="F7" s="43">
+      <c r="F7" s="45">
         <v>0</v>
       </c>
     </row>
@@ -1513,10 +1513,10 @@
       <c r="B8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="44"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="46"/>
     </row>
     <row r="9" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
@@ -1525,16 +1525,16 @@
       <c r="B9" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="53">
+      <c r="C9" s="42">
         <v>2</v>
       </c>
-      <c r="D9" s="54">
+      <c r="D9" s="55">
         <v>44327</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="55">
         <v>44328</v>
       </c>
-      <c r="F9" s="55">
+      <c r="F9" s="56">
         <v>0</v>
       </c>
     </row>
@@ -1545,10 +1545,10 @@
       <c r="B10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="55"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="56"/>
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -1557,10 +1557,10 @@
       <c r="B11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="53"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="55"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="56"/>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -1609,16 +1609,16 @@
       <c r="B14" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="53">
+      <c r="C14" s="42">
         <v>2</v>
       </c>
       <c r="D14" s="57">
         <v>44335</v>
       </c>
-      <c r="E14" s="41">
+      <c r="E14" s="43">
         <v>44336</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="45">
         <v>0</v>
       </c>
     </row>
@@ -1629,10 +1629,10 @@
       <c r="B15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="53"/>
+      <c r="C15" s="42"/>
       <c r="D15" s="58"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="46"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -1660,32 +1660,32 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="50" t="s">
+      <c r="C20" s="52" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="59" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="60"/>
-      <c r="F20" s="47">
+      <c r="F20" s="49">
         <f>SUM(F5:F15)/6</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.11666666666666665</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="C21" s="51"/>
+      <c r="C21" s="53"/>
       <c r="D21" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="48"/>
+      <c r="F21" s="50"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
-      <c r="C22" s="52"/>
+      <c r="C22" s="54"/>
       <c r="D22" s="10">
         <f>D5</f>
         <v>44321</v>
@@ -1694,7 +1694,7 @@
         <f>E14</f>
         <v>44336</v>
       </c>
-      <c r="F22" s="49"/>
+      <c r="F22" s="51"/>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C25" s="33" t="s">
@@ -1706,12 +1706,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
@@ -1727,6 +1721,12 @@
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="D20:E20"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1752,24 +1752,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G3" s="17"/>
@@ -1802,14 +1802,14 @@
         <v>1</v>
       </c>
       <c r="B5" s="9"/>
-      <c r="C5" s="45">
+      <c r="C5" s="47">
         <v>1</v>
       </c>
       <c r="D5" s="62">
         <v>44326</v>
       </c>
       <c r="E5" s="57"/>
-      <c r="F5" s="55">
+      <c r="F5" s="56">
         <v>0</v>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       <c r="C6" s="61"/>
       <c r="D6" s="63"/>
       <c r="E6" s="64"/>
-      <c r="F6" s="55"/>
+      <c r="F6" s="56"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -1831,31 +1831,31 @@
       <c r="C7" s="61"/>
       <c r="D7" s="63"/>
       <c r="E7" s="64"/>
-      <c r="F7" s="55"/>
+      <c r="F7" s="56"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>4</v>
       </c>
       <c r="B8" s="7"/>
-      <c r="C8" s="46"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="65"/>
       <c r="E8" s="58"/>
-      <c r="F8" s="55"/>
+      <c r="F8" s="56"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>5</v>
       </c>
       <c r="B9" s="9"/>
-      <c r="C9" s="45">
+      <c r="C9" s="47">
         <v>1</v>
       </c>
       <c r="D9" s="62">
         <v>44327</v>
       </c>
       <c r="E9" s="57"/>
-      <c r="F9" s="55">
+      <c r="F9" s="56">
         <v>0</v>
       </c>
     </row>
@@ -1867,7 +1867,7 @@
       <c r="C10" s="61"/>
       <c r="D10" s="63"/>
       <c r="E10" s="64"/>
-      <c r="F10" s="55"/>
+      <c r="F10" s="56"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -1877,31 +1877,31 @@
       <c r="C11" s="61"/>
       <c r="D11" s="63"/>
       <c r="E11" s="64"/>
-      <c r="F11" s="55"/>
+      <c r="F11" s="56"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>8</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="46"/>
+      <c r="C12" s="48"/>
       <c r="D12" s="65"/>
       <c r="E12" s="58"/>
-      <c r="F12" s="55"/>
+      <c r="F12" s="56"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>9</v>
       </c>
       <c r="B13" s="9"/>
-      <c r="C13" s="45">
+      <c r="C13" s="47">
         <v>1</v>
       </c>
       <c r="D13" s="62">
         <v>44328</v>
       </c>
       <c r="E13" s="57"/>
-      <c r="F13" s="55">
+      <c r="F13" s="56">
         <v>0</v>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       <c r="C14" s="61"/>
       <c r="D14" s="63"/>
       <c r="E14" s="64"/>
-      <c r="F14" s="55"/>
+      <c r="F14" s="56"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
@@ -1923,31 +1923,31 @@
       <c r="C15" s="61"/>
       <c r="D15" s="63"/>
       <c r="E15" s="64"/>
-      <c r="F15" s="55"/>
+      <c r="F15" s="56"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>12</v>
       </c>
       <c r="B16" s="7"/>
-      <c r="C16" s="46"/>
+      <c r="C16" s="48"/>
       <c r="D16" s="65"/>
       <c r="E16" s="58"/>
-      <c r="F16" s="55"/>
+      <c r="F16" s="56"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>13</v>
       </c>
       <c r="B17" s="9"/>
-      <c r="C17" s="45">
+      <c r="C17" s="47">
         <v>1</v>
       </c>
       <c r="D17" s="62">
         <v>44329</v>
       </c>
       <c r="E17" s="57"/>
-      <c r="F17" s="55">
+      <c r="F17" s="56">
         <v>0</v>
       </c>
     </row>
@@ -1959,7 +1959,7 @@
       <c r="C18" s="61"/>
       <c r="D18" s="63"/>
       <c r="E18" s="64"/>
-      <c r="F18" s="55"/>
+      <c r="F18" s="56"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
@@ -1969,31 +1969,31 @@
       <c r="C19" s="61"/>
       <c r="D19" s="63"/>
       <c r="E19" s="64"/>
-      <c r="F19" s="55"/>
+      <c r="F19" s="56"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>16</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="46"/>
+      <c r="C20" s="48"/>
       <c r="D20" s="65"/>
       <c r="E20" s="58"/>
-      <c r="F20" s="55"/>
+      <c r="F20" s="56"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>13</v>
       </c>
       <c r="B21" s="9"/>
-      <c r="C21" s="45">
+      <c r="C21" s="47">
         <v>1</v>
       </c>
       <c r="D21" s="62">
         <v>44330</v>
       </c>
       <c r="E21" s="57"/>
-      <c r="F21" s="55">
+      <c r="F21" s="56">
         <v>0</v>
       </c>
     </row>
@@ -2005,7 +2005,7 @@
       <c r="C22" s="61"/>
       <c r="D22" s="63"/>
       <c r="E22" s="64"/>
-      <c r="F22" s="55"/>
+      <c r="F22" s="56"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
@@ -2015,17 +2015,17 @@
       <c r="C23" s="61"/>
       <c r="D23" s="63"/>
       <c r="E23" s="64"/>
-      <c r="F23" s="55"/>
+      <c r="F23" s="56"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>16</v>
       </c>
       <c r="B24" s="7"/>
-      <c r="C24" s="46"/>
+      <c r="C24" s="48"/>
       <c r="D24" s="65"/>
       <c r="E24" s="58"/>
-      <c r="F24" s="55"/>
+      <c r="F24" s="56"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
@@ -2054,32 +2054,32 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
-      <c r="C29" s="50" t="s">
+      <c r="C29" s="52" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="14" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="15"/>
-      <c r="F29" s="47">
+      <c r="F29" s="49">
         <f>SUM(F5:F8)/6</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="5"/>
-      <c r="C30" s="51"/>
+      <c r="C30" s="53"/>
       <c r="D30" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="48"/>
+      <c r="F30" s="50"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="6"/>
-      <c r="C31" s="52"/>
+      <c r="C31" s="54"/>
       <c r="D31" s="10">
         <f>D5</f>
         <v>44326</v>
@@ -2088,21 +2088,10 @@
         <f>D17</f>
         <v>44329</v>
       </c>
-      <c r="F31" s="49"/>
+      <c r="F31" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="D21:E24"/>
-    <mergeCell ref="F21:F24"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:E16"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:E20"/>
-    <mergeCell ref="F17:F20"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="D9:E12"/>
     <mergeCell ref="F9:F12"/>
@@ -2111,6 +2100,17 @@
     <mergeCell ref="C5:C8"/>
     <mergeCell ref="D5:E8"/>
     <mergeCell ref="F5:F8"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:E16"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="C17:C20"/>
+    <mergeCell ref="D17:E20"/>
+    <mergeCell ref="F17:F20"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D21:E24"/>
+    <mergeCell ref="F21:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se agregó calendar y barra superir admin
</commit_message>
<xml_diff>
--- a/requerimientos/cronograma.xlsx
+++ b/requerimientos/cronograma.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\oelt_v2\requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A22154-02B4-4E2F-BF79-50A12D4047CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FEF65A-7845-4036-9B2F-B01F1EB1D952}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Semana 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Semana 2" sheetId="2" r:id="rId2"/>
+    <sheet name="OELT" sheetId="2" r:id="rId1"/>
+    <sheet name="BIOMASTR" sheetId="1" r:id="rId2"/>
     <sheet name="Hoja1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
   <si>
     <t>Item</t>
   </si>
@@ -178,8 +178,7 @@
 4. Catálogo (OK)
 5. Capacitación(cursos, diplomados)(OK)
 6. Intranet(OK)
-7. Aula Virtual
-8. Contacto(OK)
+7. Contacto(OK)
 </t>
     </r>
     <r>
@@ -204,6 +203,21 @@
       <t xml:space="preserve"> agregar las redes sociales, email y celular de la empresa OELT</t>
     </r>
   </si>
+  <si>
+    <t>a. Implementar menu arriba admin
+b. Implementar vistas a la sección admin
+1. inicio
+2. Areas
+3. Cursos
+4. Cronogramas
+5. Certificados
+6. Estudiantes
+7. Profesores</t>
+  </si>
+  <si>
+    <t>Aplicación web: Adaptar el código existente con la nueva versión MVC
+1. Consulta de certificado (buscar por código o dni)</t>
+  </si>
 </sst>
 </file>
 
@@ -554,7 +568,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -704,15 +718,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -790,15 +795,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -873,7 +869,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="25" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -902,19 +898,19 @@
     <xf numFmtId="14" fontId="24" fillId="25" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -923,7 +919,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -971,10 +967,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -983,85 +979,79 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="24" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="24" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="26" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="25" fillId="26" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="26" fillId="24" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="26" fillId="24" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="26" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="26" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="25" fillId="26" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="26" fillId="24" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1386,11 +1376,325 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978140A5-7C6C-47A4-8352-734FB3DF76C6}">
+  <dimension ref="A1:J21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="118" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="45">
+        <v>5</v>
+      </c>
+      <c r="D5" s="41">
+        <v>44326</v>
+      </c>
+      <c r="E5" s="41">
+        <v>44330</v>
+      </c>
+      <c r="F5" s="55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="150" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>2</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="61"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="55"/>
+    </row>
+    <row r="7" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>5</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="45">
+        <v>2</v>
+      </c>
+      <c r="D7" s="54">
+        <v>44333</v>
+      </c>
+      <c r="E7" s="54">
+        <v>44335</v>
+      </c>
+      <c r="F7" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>6</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="61"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55"/>
+    </row>
+    <row r="9" spans="1:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>9</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="45">
+        <v>3</v>
+      </c>
+      <c r="D9" s="54">
+        <v>44336</v>
+      </c>
+      <c r="E9" s="54">
+        <v>44340</v>
+      </c>
+      <c r="F9" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="61"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="55"/>
+    </row>
+    <row r="11" spans="1:10" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>13</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="45">
+        <v>2</v>
+      </c>
+      <c r="D11" s="54">
+        <v>44341</v>
+      </c>
+      <c r="E11" s="54">
+        <v>44342</v>
+      </c>
+      <c r="F11" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="120" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>14</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="61"/>
+      <c r="D12" s="54"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>13</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="53">
+        <v>1</v>
+      </c>
+      <c r="D13" s="62">
+        <v>44343</v>
+      </c>
+      <c r="E13" s="56"/>
+      <c r="F13" s="55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>14</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="53"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="55"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="13">
+        <f>SUM(C5:C14)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="47">
+        <f>SUM(F5:F14)/5</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="48"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="10">
+        <f>D5</f>
+        <v>44326</v>
+      </c>
+      <c r="E21" s="11">
+        <v>44344</v>
+      </c>
+      <c r="F21" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="23">
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="109" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F8"/>
+    <sheetView zoomScale="109" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,24 +1707,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -1461,80 +1765,80 @@
       <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="42">
+      <c r="C5" s="53">
         <v>2</v>
       </c>
-      <c r="D5" s="43">
+      <c r="D5" s="41">
         <v>44321</v>
       </c>
-      <c r="E5" s="43">
+      <c r="E5" s="41">
         <v>44322</v>
       </c>
-      <c r="F5" s="45">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+      <c r="F5" s="43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>2</v>
       </c>
       <c r="B6" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="46"/>
-    </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="C6" s="53"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="44"/>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>3</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="47">
+        <v>29</v>
+      </c>
+      <c r="C7" s="45">
         <v>2</v>
       </c>
-      <c r="D7" s="43">
-        <v>44323</v>
-      </c>
-      <c r="E7" s="43">
-        <v>44326</v>
-      </c>
-      <c r="F7" s="45">
+      <c r="D7" s="41">
+        <v>44333</v>
+      </c>
+      <c r="E7" s="41">
+        <v>44334</v>
+      </c>
+      <c r="F7" s="43">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>4</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="46"/>
-    </row>
-    <row r="9" spans="1:10" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="C8" s="46"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="44"/>
+    </row>
+    <row r="9" spans="1:10" s="3" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>5</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="42">
+        <v>19</v>
+      </c>
+      <c r="C9" s="53">
         <v>2</v>
       </c>
-      <c r="D9" s="55">
+      <c r="D9" s="54">
         <v>44327</v>
       </c>
-      <c r="E9" s="55">
+      <c r="E9" s="54">
         <v>44328</v>
       </c>
-      <c r="F9" s="56">
+      <c r="F9" s="55">
         <v>0</v>
       </c>
     </row>
@@ -1545,10 +1849,10 @@
       <c r="B10" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="55"/>
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
@@ -1557,10 +1861,10 @@
       <c r="B11" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="56"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -1609,16 +1913,16 @@
       <c r="B14" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="42">
+      <c r="C14" s="53">
         <v>2</v>
       </c>
-      <c r="D14" s="57">
+      <c r="D14" s="56">
         <v>44335</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="41">
         <v>44336</v>
       </c>
-      <c r="F14" s="45">
+      <c r="F14" s="43">
         <v>0</v>
       </c>
     </row>
@@ -1629,10 +1933,10 @@
       <c r="B15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="46"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="44"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
@@ -1660,32 +1964,32 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
-      <c r="C20" s="52" t="s">
+      <c r="C20" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="D20" s="59" t="s">
+      <c r="D20" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="60"/>
-      <c r="F20" s="49">
+      <c r="E20" s="59"/>
+      <c r="F20" s="47">
         <f>SUM(F5:F15)/6</f>
-        <v>0.11666666666666665</v>
+        <v>0.16666666666666666</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
-      <c r="C21" s="53"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="8" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="50"/>
+      <c r="F21" s="48"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
-      <c r="C22" s="54"/>
+      <c r="C22" s="52"/>
       <c r="D22" s="10">
         <f>D5</f>
         <v>44321</v>
@@ -1694,7 +1998,7 @@
         <f>E14</f>
         <v>44336</v>
       </c>
-      <c r="F22" s="51"/>
+      <c r="F22" s="49"/>
     </row>
     <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C25" s="33" t="s">
@@ -1706,6 +2010,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
@@ -1721,398 +2031,9 @@
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="D20:E20"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978140A5-7C6C-47A4-8352-734FB3DF76C6}">
-  <dimension ref="A1:J31"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="71.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>1</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="47">
-        <v>1</v>
-      </c>
-      <c r="D5" s="62">
-        <v>44326</v>
-      </c>
-      <c r="E5" s="57"/>
-      <c r="F5" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>2</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="56"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>3</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="56"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>4</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="56"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>5</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="47">
-        <v>1</v>
-      </c>
-      <c r="D9" s="62">
-        <v>44327</v>
-      </c>
-      <c r="E9" s="57"/>
-      <c r="F9" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>6</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="56"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="56"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>8</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="56"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
-        <v>9</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="47">
-        <v>1</v>
-      </c>
-      <c r="D13" s="62">
-        <v>44328</v>
-      </c>
-      <c r="E13" s="57"/>
-      <c r="F13" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
-        <v>10</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="56"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>11</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="56"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
-        <v>12</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="65"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="56"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
-        <v>13</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="47">
-        <v>1</v>
-      </c>
-      <c r="D17" s="62">
-        <v>44329</v>
-      </c>
-      <c r="E17" s="57"/>
-      <c r="F17" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>14</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="56"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>15</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="64"/>
-      <c r="F19" s="56"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>16</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="56"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>13</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="47">
-        <v>1</v>
-      </c>
-      <c r="D21" s="62">
-        <v>44330</v>
-      </c>
-      <c r="E21" s="57"/>
-      <c r="F21" s="56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>14</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="56"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>15</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="56"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
-        <v>16</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="56"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="22"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="13">
-        <f>SUM(C5:C20)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="5"/>
-      <c r="C29" s="52" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="15"/>
-      <c r="F29" s="49">
-        <f>SUM(F5:F8)/6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="5"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F30" s="50"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="54"/>
-      <c r="D31" s="10">
-        <f>D5</f>
-        <v>44326</v>
-      </c>
-      <c r="E31" s="11">
-        <f>D17</f>
-        <v>44329</v>
-      </c>
-      <c r="F31" s="51"/>
-    </row>
-  </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:E12"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:E8"/>
-    <mergeCell ref="F5:F8"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:E16"/>
-    <mergeCell ref="F13:F16"/>
-    <mergeCell ref="C17:C20"/>
-    <mergeCell ref="D17:E20"/>
-    <mergeCell ref="F17:F20"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="D21:E24"/>
-    <mergeCell ref="F21:F24"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>